<commit_message>
CST EB updated run files
</commit_message>
<xml_diff>
--- a/Run_Files/Figure1/lhs_settings_input.xlsx
+++ b/Run_Files/Figure1/lhs_settings_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kthng\Google Drive\ARNOLD LAB GOOGDRI\Bacterial Vaginosis\Aim2_Interspecies_Interactions\numerical_interspecies\analyze_probiotic_add\2021-03-03-Compare-LHS-alpha-SS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/ARNOLD LAB GOOGDRI/Bacterial Vaginosis/Aim3_Clinical_Interspecies/2022-05-02-Manu-Update-Val-all-param-LHS/Figure1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C76272-5B68-4E89-BFD1-B0B1EBF6DD3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D1E2DA-8A86-E244-BAEA-3812A0E8A987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -98,10 +98,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,10 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,18 +464,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="4" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,53 +489,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C5">
         <v>-0.04</v>
       </c>
       <c r="D5">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -543,7 +559,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,7 +573,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -571,19 +587,21 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C9">
         <v>-0.04</v>
       </c>
       <c r="D9">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -597,7 +615,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -612,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -626,16 +644,18 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C13">
         <v>-0.04</v>
       </c>
       <c r="D13">
-        <v>-0.04</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -647,18 +667,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="4" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,37 +692,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update species names in input LHS file
</commit_message>
<xml_diff>
--- a/Run_Files/Figure1/lhs_settings_input.xlsx
+++ b/Run_Files/Figure1/lhs_settings_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/ARNOLD LAB GOOGDRI/Bacterial Vaginosis/Aim3_Clinical_Interspecies/2022-05-02-Manu-Update-Val-all-param-LHS/Figure1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chlee/Documents/MATLAB/CST_ODE/Run_Files/Figure1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D1E2DA-8A86-E244-BAEA-3812A0E8A987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88775168-EFF0-1448-B7D1-F856A9997486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="21600" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -37,15 +37,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>k_{grow}-BV1</t>
-  </si>
-  <si>
-    <t>k_{grow}-LB1</t>
-  </si>
-  <si>
-    <t>k_{grow}-P</t>
-  </si>
-  <si>
     <t>distribution</t>
   </si>
   <si>
@@ -55,43 +46,52 @@
     <t>value 2</t>
   </si>
   <si>
-    <t>\alpha_{BV1-&gt;BV1}</t>
-  </si>
-  <si>
-    <t>\alpha_{BV1-&gt;LB1}</t>
-  </si>
-  <si>
-    <t>\alpha_{BV1-&gt;P}</t>
-  </si>
-  <si>
-    <t>\alpha_{LB1-&gt;BV1}</t>
-  </si>
-  <si>
-    <t>\alpha_{LB1-&gt;LB1}</t>
-  </si>
-  <si>
-    <t>\alpha_{LB1-&gt;P}</t>
-  </si>
-  <si>
-    <t>\alpha_{P-&gt;BV1}</t>
-  </si>
-  <si>
-    <t>\alpha_{P-&gt;LB1}</t>
-  </si>
-  <si>
-    <t>\alpha_{P-&gt;P}</t>
-  </si>
-  <si>
-    <t>BV1</t>
-  </si>
-  <si>
-    <t>LB1</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>u</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>oLB</t>
+  </si>
+  <si>
+    <t>k_{grow}-NO</t>
+  </si>
+  <si>
+    <t>k_{grow}-Li</t>
+  </si>
+  <si>
+    <t>k_{grow}-oLB</t>
+  </si>
+  <si>
+    <t>\alpha_{NO-&gt;NO}</t>
+  </si>
+  <si>
+    <t>\alpha_{NO-&gt;Li}</t>
+  </si>
+  <si>
+    <t>\alpha_{NO-&gt;oLB}</t>
+  </si>
+  <si>
+    <t>\alpha_{Li-&gt;NO}</t>
+  </si>
+  <si>
+    <t>\alpha_{Li-&gt;Li}</t>
+  </si>
+  <si>
+    <t>\alpha_{Li-&gt;oLB}</t>
+  </si>
+  <si>
+    <t>\alpha_{oLB-&gt;NO}</t>
+  </si>
+  <si>
+    <t>\alpha_{oLB-&gt;Li}</t>
+  </si>
+  <si>
+    <t>\alpha_{oLB-&gt;oLB}</t>
   </si>
 </sst>
 </file>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -480,21 +480,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0.1</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0.1</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>-0.04</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>-0.12</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>-0.12</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>-0.12</v>
@@ -589,10 +589,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>-0.04</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>-0.12</v>
@@ -617,10 +617,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f>C10</f>
@@ -632,10 +632,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>-0.12</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>-0.04</v>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="174" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,18 +683,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>20</v>

</xml_diff>